<commit_message>
Added the rest of vendor records
</commit_message>
<xml_diff>
--- a/eProcurement_template.xlsx
+++ b/eProcurement_template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nappiah\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ofosu\OneDrive\Documents\Projects\DigiProc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:101_{20995965-AB1B-464E-80E2-BBDAF8AF5476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ItemCategory" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="Vendor_List" sheetId="3" r:id="rId3"/>
     <sheet name="VendorType" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="281">
   <si>
     <t>CategoryID</t>
   </si>
@@ -878,12 +877,15 @@
   </si>
   <si>
     <t>Gifty Sowah</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0000000000000"/>
     <numFmt numFmtId="165" formatCode="0000000000"/>
@@ -1254,7 +1256,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A28:C29"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
@@ -1297,7 +1299,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F21CA0-AEB3-4714-981B-7437F4F05220}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1364,11 +1366,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F36BCA-22E2-42D6-A32B-64D6FCED4655}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1383,7 +1385,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>4</v>
+        <v>280</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>14</v>
@@ -2996,10 +2998,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G32" r:id="rId1" xr:uid="{8FA6854F-CEC3-4AD9-A01E-72CA9776E964}"/>
-    <hyperlink ref="F107" r:id="rId2" xr:uid="{1850884F-C2F4-4948-AB4A-FBACA30B00AD}"/>
-    <hyperlink ref="F108" r:id="rId3" xr:uid="{1C10B546-AD92-435B-927C-F5F01306F538}"/>
-    <hyperlink ref="F109" r:id="rId4" xr:uid="{32387564-B0CB-4FDA-BD48-83D060321AB8}"/>
+    <hyperlink ref="G32" r:id="rId1"/>
+    <hyperlink ref="F107" r:id="rId2"/>
+    <hyperlink ref="F108" r:id="rId3"/>
+    <hyperlink ref="F109" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId5"/>
@@ -3007,7 +3009,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A64730F6-BAD7-4AC8-ACC2-7D9A2B72E5B6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>